<commit_message>
created buggy poorly-coded method flipInterface(). It saves time instead of making two interfaces.
</commit_message>
<xml_diff>
--- a/TagsClassified.xlsx
+++ b/TagsClassified.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IV Class" sheetId="10" r:id="rId1"/>
     <sheet name="IV Class^2" sheetId="12" r:id="rId2"/>
     <sheet name="PV Class" sheetId="11" r:id="rId3"/>
     <sheet name="PV Class^2" sheetId="13" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="15" r:id="rId6"/>
+    <sheet name="N Class" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IV Class'!$D$1:$J$178</definedName>
@@ -344,8 +343,61 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>omar</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>omar:
+This table is severely outdated. It contains many mistakes that were fixed in both its parent: file "StemsTagsComments.xlsx"; and its children: sheet "IV_Class^2" and file "BuckTagRules.xls".
+It is only kept for reference.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>تفرق أوله همزة أو لا فقط إذا كان حرف مضارعته مفتوحا، ويجوز أن يكون ألفا</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Every modified stem should be mapped back to its original unmodified form, a "سليم". However, some stems map to two different "سليم"s, like يعدو and يسعى both map to one form where their last letter is deleted to get suffix ون.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2817" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="238">
   <si>
     <t>PV_V</t>
   </si>
@@ -861,6 +913,204 @@
   </si>
   <si>
     <t>آخره همزة</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N/ap</t>
+  </si>
+  <si>
+    <t>N/ap_L</t>
+  </si>
+  <si>
+    <t>N/At</t>
+  </si>
+  <si>
+    <t>N/At_L</t>
+  </si>
+  <si>
+    <t>N_L</t>
+  </si>
+  <si>
+    <t>N-|</t>
+  </si>
+  <si>
+    <t>N-|t</t>
+  </si>
+  <si>
+    <t>N0</t>
+  </si>
+  <si>
+    <t>N0_L</t>
+  </si>
+  <si>
+    <t>N0_Nh</t>
+  </si>
+  <si>
+    <t>N0_Nh_L</t>
+  </si>
+  <si>
+    <t>N0_Nhy</t>
+  </si>
+  <si>
+    <t>N0F</t>
+  </si>
+  <si>
+    <t>N0F_Nh</t>
+  </si>
+  <si>
+    <t>Nall</t>
+  </si>
+  <si>
+    <t>Nall_L</t>
+  </si>
+  <si>
+    <t>NAn_Nayn</t>
+  </si>
+  <si>
+    <t>NAn_Nayn_L</t>
+  </si>
+  <si>
+    <t>Nap</t>
+  </si>
+  <si>
+    <t>N-ap</t>
+  </si>
+  <si>
+    <t>Nap_L</t>
+  </si>
+  <si>
+    <t>N-ap_L</t>
+  </si>
+  <si>
+    <t>NapAt</t>
+  </si>
+  <si>
+    <t>NapAt_L</t>
+  </si>
+  <si>
+    <t>Napdu</t>
+  </si>
+  <si>
+    <t>Napdu_L</t>
+  </si>
+  <si>
+    <t>NAt</t>
+  </si>
+  <si>
+    <t>NAt_L</t>
+  </si>
+  <si>
+    <t>Nayn</t>
+  </si>
+  <si>
+    <t>Ndip</t>
+  </si>
+  <si>
+    <t>Ndip_L</t>
+  </si>
+  <si>
+    <t>Ndu</t>
+  </si>
+  <si>
+    <t>Ndu_L</t>
+  </si>
+  <si>
+    <t>NduAt</t>
+  </si>
+  <si>
+    <t>NduAt_L</t>
+  </si>
+  <si>
+    <t>Nel</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>NF_Nhy</t>
+  </si>
+  <si>
+    <t>Nh</t>
+  </si>
+  <si>
+    <t>Nh_L</t>
+  </si>
+  <si>
+    <t>Nh_Niyn</t>
+  </si>
+  <si>
+    <t>Nh_Nuwn</t>
+  </si>
+  <si>
+    <t>Nhy</t>
+  </si>
+  <si>
+    <t>Nhy_L</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>Nprop</t>
+  </si>
+  <si>
+    <t>Numb</t>
+  </si>
+  <si>
+    <t>Nuwn_Niyn</t>
+  </si>
+  <si>
+    <t>Nuwn_Niyn_L</t>
+  </si>
+  <si>
+    <t>اسم</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Feminine, able to become</t>
+  </si>
+  <si>
+    <t>Singular/Dual/Plural</t>
+  </si>
+  <si>
+    <t>Dual, able to become</t>
+  </si>
+  <si>
+    <t>Rg. Masc. Pl., able to become</t>
+  </si>
+  <si>
+    <t>Rg. Femn. Pl., able to become</t>
+  </si>
+  <si>
+    <t>بتاء مربوطة</t>
+  </si>
+  <si>
+    <t>مذكر</t>
+  </si>
+  <si>
+    <t>لا</t>
+  </si>
+  <si>
+    <t>مفرد</t>
+  </si>
+  <si>
+    <t>نعم</t>
+  </si>
+  <si>
+    <t>Lam, First is</t>
+  </si>
+  <si>
+    <t>مفرد أو مكسر</t>
+  </si>
+  <si>
+    <t>"أ"</t>
+  </si>
+  <si>
+    <t>مؤنث</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1886,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1796,6 +2046,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2211,7 +2464,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8005,10 +8258,10 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9157,11 +9410,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O129"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10367,32 +10620,32 @@
       </c>
       <c r="M39" s="59"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A40" s="64" t="s">
+    <row r="40" spans="1:13">
+      <c r="A40" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="58">
+      <c r="B40" s="57">
         <v>152</v>
       </c>
-      <c r="C40" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="24" t="s">
+      <c r="C40" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F40" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I40" s="25" t="s">
+      <c r="F40" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="15" t="s">
         <v>98</v>
       </c>
       <c r="J40" s="16" t="s">
@@ -10736,32 +10989,32 @@
       </c>
       <c r="M50" s="59"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A51" s="64" t="s">
+    <row r="51" spans="1:13">
+      <c r="A51" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="58">
+      <c r="B51" s="57">
         <v>41</v>
       </c>
-      <c r="C51" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="24" t="s">
+      <c r="C51" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F51" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H51" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I51" s="25" t="s">
+      <c r="F51" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I51" s="15" t="s">
         <v>85</v>
       </c>
       <c r="J51" s="16" t="s">
@@ -10875,32 +11128,32 @@
       <c r="L55" s="11"/>
       <c r="M55" s="59"/>
     </row>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A56" s="64" t="s">
+    <row r="56" spans="1:13">
+      <c r="A56" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="58">
+      <c r="B56" s="57">
         <v>3</v>
       </c>
-      <c r="C56" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="24" t="s">
+      <c r="C56" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="24" t="s">
+      <c r="E56" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="F56" s="25" t="s">
+      <c r="F56" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H56" s="24" t="s">
+      <c r="G56" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H56" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I56" s="25" t="s">
+      <c r="I56" s="15" t="s">
         <v>98</v>
       </c>
       <c r="J56" s="16" t="s">
@@ -10912,32 +11165,32 @@
       </c>
       <c r="M56" s="59"/>
     </row>
-    <row r="57" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A57" s="64" t="s">
+    <row r="57" spans="1:13">
+      <c r="A57" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="B57" s="58">
+      <c r="B57" s="57">
         <v>3</v>
       </c>
-      <c r="C57" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="24" t="s">
+      <c r="C57" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="24" t="s">
+      <c r="E57" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="F57" s="25" t="s">
+      <c r="F57" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G57" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" s="24" t="s">
+      <c r="G57" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H57" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="I57" s="25" t="s">
+      <c r="I57" s="15" t="s">
         <v>98</v>
       </c>
       <c r="J57" s="16" t="s">
@@ -11051,32 +11304,32 @@
       <c r="L61" s="11"/>
       <c r="M61" s="59"/>
     </row>
-    <row r="62" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A62" s="64" t="s">
+    <row r="62" spans="1:13">
+      <c r="A62" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="58">
+      <c r="B62" s="57">
         <v>29</v>
       </c>
-      <c r="C62" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D62" s="24" t="s">
+      <c r="C62" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="25" t="s">
+      <c r="F62" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G62" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H62" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I62" s="25" t="s">
+      <c r="G62" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I62" s="15" t="s">
         <v>98</v>
       </c>
       <c r="J62" s="16" t="s">
@@ -11190,32 +11443,32 @@
       <c r="L66" s="11"/>
       <c r="M66" s="59"/>
     </row>
-    <row r="67" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A67" s="64" t="s">
+    <row r="67" spans="1:13">
+      <c r="A67" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="58">
+      <c r="B67" s="57">
         <v>5</v>
       </c>
-      <c r="C67" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D67" s="24" t="s">
+      <c r="C67" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E67" s="24" t="s">
+      <c r="E67" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F67" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G67" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H67" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I67" s="25" t="s">
+      <c r="G67" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I67" s="15" t="s">
         <v>85</v>
       </c>
       <c r="J67" s="16" t="s">
@@ -11329,32 +11582,32 @@
       <c r="L71" s="11"/>
       <c r="M71" s="59"/>
     </row>
-    <row r="72" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A72" s="64" t="s">
+    <row r="72" spans="1:13">
+      <c r="A72" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="58">
+      <c r="B72" s="57">
         <v>53</v>
       </c>
-      <c r="C72" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D72" s="24" t="s">
+      <c r="C72" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E72" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F72" s="25" t="s">
+      <c r="F72" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G72" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H72" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I72" s="25" t="s">
+      <c r="G72" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I72" s="15" t="s">
         <v>98</v>
       </c>
       <c r="J72" s="16" t="s">
@@ -11468,32 +11721,32 @@
       <c r="L76" s="11"/>
       <c r="M76" s="59"/>
     </row>
-    <row r="77" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A77" s="64" t="s">
+    <row r="77" spans="1:13">
+      <c r="A77" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="58">
+      <c r="B77" s="57">
         <v>15</v>
       </c>
-      <c r="C77" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D77" s="24" t="s">
+      <c r="C77" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E77" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F77" s="25" t="s">
+      <c r="F77" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G77" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H77" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I77" s="25" t="s">
+      <c r="G77" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I77" s="15" t="s">
         <v>85</v>
       </c>
       <c r="J77" s="16" t="s">
@@ -12644,1229 +12897,1277 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="E1" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A2" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="E2" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="16" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8818</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="1">
+        <v>730</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1787</v>
+      </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" t="s">
+        <v>231</v>
+      </c>
+      <c r="I4" t="s">
+        <v>233</v>
+      </c>
+      <c r="J4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="1">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" t="s">
+        <v>236</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" t="s">
+        <v>231</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1595</v>
+      </c>
+      <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" t="s">
+        <v>231</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="1">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="J9" t="s">
+        <v>231</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="1">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="1">
+        <v>146</v>
+      </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="J11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5597</v>
+      </c>
+      <c r="C12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="J12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="1">
+        <v>829</v>
+      </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3808</v>
+      </c>
+      <c r="C14" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="70" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2482</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1928</v>
+      </c>
+      <c r="C16" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" t="s">
+        <v>231</v>
+      </c>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1726</v>
+      </c>
+      <c r="C17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="J17" t="s">
+        <v>231</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="70" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1495</v>
+      </c>
+      <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="1">
+        <v>264</v>
+      </c>
+      <c r="C19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" t="s">
+        <v>231</v>
+      </c>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2485</v>
+      </c>
+      <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="I20" s="5"/>
+      <c r="J20" t="s">
+        <v>231</v>
+      </c>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2050</v>
+      </c>
+      <c r="C21" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" t="s">
+        <v>231</v>
+      </c>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1617</v>
+      </c>
+      <c r="C22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="1">
+        <v>818</v>
+      </c>
+      <c r="C23" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="70" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="1">
+        <v>279</v>
+      </c>
+      <c r="C24" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="1">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1277</v>
+      </c>
+      <c r="C26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="J26" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="1">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" s="1">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1761</v>
+      </c>
+      <c r="C29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="1">
+        <v>515</v>
+      </c>
+      <c r="C30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="J30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2405</v>
+      </c>
+      <c r="C31" t="s">
+        <v>222</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" s="1">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>222</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32" s="3"/>
+      <c r="J32" t="s">
+        <v>231</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="1">
+        <v>288</v>
+      </c>
+      <c r="C33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="70"/>
+      <c r="B34" s="1"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="70"/>
+      <c r="B35" s="1"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="70"/>
+      <c r="B36" s="1"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="70"/>
+      <c r="B37" s="1"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="1">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G38" t="s">
+        <v>233</v>
+      </c>
+      <c r="H38" t="s">
+        <v>231</v>
+      </c>
+      <c r="I38" t="s">
+        <v>233</v>
+      </c>
+      <c r="J38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="1">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>222</v>
+      </c>
+      <c r="D39" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" t="s">
+        <v>231</v>
+      </c>
+      <c r="H39" t="s">
+        <v>231</v>
+      </c>
+      <c r="I39" t="s">
+        <v>233</v>
+      </c>
+      <c r="J39" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="1">
+        <v>210</v>
+      </c>
+      <c r="C40" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" t="s">
+        <v>231</v>
+      </c>
+      <c r="H40" t="s">
+        <v>231</v>
+      </c>
+      <c r="I40" t="s">
+        <v>231</v>
+      </c>
+      <c r="J40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A41" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" s="1">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="I41" s="5"/>
+      <c r="J41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" s="1">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" t="s">
+        <v>233</v>
+      </c>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="70" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="1">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>222</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" t="s">
+        <v>233</v>
+      </c>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="J44" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" s="1">
         <v>120</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A4" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A5" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A6" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="60" t="s">
+      <c r="C45" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" t="s">
+        <v>233</v>
+      </c>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="B46" s="1">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
+        <v>222</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" t="s">
+        <v>233</v>
+      </c>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" t="s">
+        <v>233</v>
+      </c>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A48" s="70" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A7" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="62" t="s">
+      <c r="C48" t="s">
+        <v>222</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" t="s">
+        <v>233</v>
+      </c>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>222</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="I49" s="5"/>
+      <c r="J49" t="s">
+        <v>233</v>
+      </c>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" s="1">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" t="s">
+        <v>233</v>
+      </c>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="70" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="1">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>222</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" t="s">
+        <v>233</v>
+      </c>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>222</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="J52" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" s="1">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
+        <v>222</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A54" s="70" t="s">
+        <v>216</v>
+      </c>
+      <c r="B54" s="1">
         <v>46</v>
       </c>
-      <c r="F7" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A8" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A9" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A10" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A11" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="E11" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A12" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="E12" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A13" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="E13" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A14" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A15" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="E15" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="60" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A16" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="60" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A19" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="E19" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A21" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A22" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="E22" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A23" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A24" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="60" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A28" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A29" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="E29" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A30" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="E32" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E36" s="65"/>
-    </row>
-    <row r="37" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E37" s="65"/>
-    </row>
-    <row r="43" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E43" s="65"/>
-    </row>
-    <row r="44" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E44" s="65"/>
-    </row>
-    <row r="47" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E47" s="65"/>
-    </row>
-    <row r="48" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E48" s="65"/>
-    </row>
-    <row r="60" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E60" s="65"/>
-    </row>
-    <row r="63" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E63" s="65"/>
-    </row>
-    <row r="64" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E64" s="65"/>
-    </row>
-    <row r="65" spans="5:5">
-      <c r="E65" s="60"/>
-    </row>
-    <row r="66" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E66" s="65"/>
-    </row>
-    <row r="67" spans="5:5" ht="15.75" thickBot="1">
-      <c r="E67" s="65"/>
+      <c r="C54" t="s">
+        <v>222</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A55" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A56" s="6"/>
+      <c r="B56" s="1"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A57" s="6"/>
+      <c r="B57" s="1"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A58" s="6"/>
+      <c r="B58" s="1"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A59" s="6"/>
+      <c r="B59" s="1"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A60" s="6"/>
+      <c r="B60" s="1"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A61" s="6"/>
+      <c r="B61" s="1"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A62" s="6"/>
+      <c r="B62" s="1"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A63" s="6"/>
+      <c r="B63" s="1"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A64" s="6"/>
+      <c r="B64" s="1"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A65" s="6"/>
+      <c r="B65" s="1"/>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A66" s="6"/>
+      <c r="B66" s="1"/>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A67" s="6"/>
+      <c r="B67" s="1"/>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A68" s="6"/>
+      <c r="B68" s="1"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A69" s="6"/>
+      <c r="B69" s="1"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A70" s="6"/>
+      <c r="B70" s="1"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="6"/>
+      <c r="B71" s="1"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A72" s="6"/>
+      <c r="B72" s="1"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A73" s="6"/>
+      <c r="B73" s="1"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A74" s="6"/>
+      <c r="B74" s="1"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A75" s="6"/>
+      <c r="B75" s="1"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A76" s="6"/>
+      <c r="B76" s="1"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A77" s="6"/>
+      <c r="B77" s="1"/>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A78" s="6"/>
+      <c r="B78" s="1"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A79" s="6"/>
+      <c r="B79" s="1"/>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A80" s="6"/>
+      <c r="B80" s="1"/>
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A81" s="6"/>
+      <c r="B81" s="1"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A82" s="6"/>
+      <c r="B82" s="1"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A83" s="6"/>
+      <c r="B83" s="1"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A84" s="6"/>
+      <c r="B84" s="1"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A85" s="6"/>
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A86" s="6"/>
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A87" s="6"/>
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A88" s="6"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A89" s="6"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A90" s="6"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A91" s="6"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A92" s="6"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A93" s="6"/>
+      <c r="B93" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:L89">
+    <sortCondition ref="J2:J89"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
-  <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:A45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A2" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A4" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A5" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A9" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A10" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A11" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="60" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A12" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A13" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A14" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A15" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A16" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A17" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A18" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A19" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A20" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A22" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A24" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A25" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E25" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A26" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A27" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A28" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E28" s="60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A29" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" s="60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A30" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A31" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A32" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A33" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A34" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A35" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A36" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="60" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A37" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E37" s="60" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A38" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A39" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A40" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A41" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A42" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A43" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E43" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A44" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E44" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>